<commit_message>
add slideshow to the header and modifiy the navigation bar
</commit_message>
<xml_diff>
--- a/src/assets/translationsfile.xlsx
+++ b/src/assets/translationsfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angular\franchinets-website\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43490A2-CCDA-4A66-94E7-1354DF9DE1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5585EE91-57FE-44D3-BAD2-EA14AB4FC07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2B2C88A7-9330-48F1-B64D-E4D3C6631A5B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -86,15 +86,9 @@
     <t>About</t>
   </si>
   <si>
-    <t>Home</t>
-  </si>
-  <si>
     <t>À Propos</t>
   </si>
   <si>
-    <t>Acceuil</t>
-  </si>
-  <si>
     <t>Aide</t>
   </si>
   <si>
@@ -128,13 +122,256 @@
     <t>franchinet_txt_header_language</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Langue</t>
-  </si>
-  <si>
     <t>BILINGUAL NUSERY AND PRIMARY SCHOOL LES FRANCHINETS</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_establishment</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_introducing</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_visitSite</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_ourBenefits</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_ourAssociation</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_praticalInfos</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_contactUs</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_inscription</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_priceList</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_internalRules</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_calendar</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_cafetaria</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_nursery</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_nurseryOperation</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_nurseryOrganization</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_personalizedAssistance</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_elementary</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_elementaryOperation</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_elementaryOrganization</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_extracurricular</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_daycareOperation</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_daycareOrganization</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_culturalAndSportingActivities</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_enieg</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_french</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_english</t>
+  </si>
+  <si>
+    <t>ENIEG</t>
+  </si>
+  <si>
+    <t>franchinet_txt_header_elementaryPersonalizedAssistance</t>
+  </si>
+  <si>
+    <t>PRESENTATION</t>
+  </si>
+  <si>
+    <t>INTRODUCING</t>
+  </si>
+  <si>
+    <t>VISITES DES LIEUX</t>
+  </si>
+  <si>
+    <t>VISIT THE SITES</t>
+  </si>
+  <si>
+    <t>OUR ASSOCIATION</t>
+  </si>
+  <si>
+    <t>NOTRE ASSOCIATION</t>
+  </si>
+  <si>
+    <t>NOS ATOUTS</t>
+  </si>
+  <si>
+    <t>OUR BENEFITS</t>
+  </si>
+  <si>
+    <t>PRACTICAL INFOS</t>
+  </si>
+  <si>
+    <t>INFOS PRACTIQUES</t>
+  </si>
+  <si>
+    <t>CONTACT US</t>
+  </si>
+  <si>
+    <t>NOUS CONTACTER</t>
+  </si>
+  <si>
+    <t>INSCRIPTION</t>
+  </si>
+  <si>
+    <t>PRICE LIST</t>
+  </si>
+  <si>
+    <t>TARIFS</t>
+  </si>
+  <si>
+    <t>INTERNAL RULES</t>
+  </si>
+  <si>
+    <t>RÈGLEMENT INTERIEUR</t>
+  </si>
+  <si>
+    <t>CALENDAR</t>
+  </si>
+  <si>
+    <t>CALENDRIER</t>
+  </si>
+  <si>
+    <t>CAFETARIA</t>
+  </si>
+  <si>
+    <t>CANTINE</t>
+  </si>
+  <si>
+    <t>NURSERY</t>
+  </si>
+  <si>
+    <t>MATERNELLE</t>
+  </si>
+  <si>
+    <t>NURSERY OPERATION</t>
+  </si>
+  <si>
+    <t>FONCTIONNEMENT DE LA MATERNELLE</t>
+  </si>
+  <si>
+    <t>NURSERY ORGANIZATION</t>
+  </si>
+  <si>
+    <t>ORGANISATION DE LA MATERNELLE</t>
+  </si>
+  <si>
+    <t>ELEMENTARY</t>
+  </si>
+  <si>
+    <t>ÉLÉMENTAIRE</t>
+  </si>
+  <si>
+    <t>ELEMENTARY OPERATION</t>
+  </si>
+  <si>
+    <t>FONCTIONNEMENT DE L'ÉLÉMENTAIRE</t>
+  </si>
+  <si>
+    <t>ELEMENTARY ORGANIZATION</t>
+  </si>
+  <si>
+    <t>ORGANISATION DE L'ÉLÉMENTAIRE</t>
+  </si>
+  <si>
+    <t>ELEMENTARY PERONALIZED ASSISTANCE</t>
+  </si>
+  <si>
+    <t>AIDE PERSONALISÉE DE L'ÉLÉMENTAIRE</t>
+  </si>
+  <si>
+    <t>NURSERY PERSONALISED ASSISTANCE</t>
+  </si>
+  <si>
+    <t>AIDE PERSONALISÉE DE LA MATERNELLE</t>
+  </si>
+  <si>
+    <t>EXTRACURRICULAR</t>
+  </si>
+  <si>
+    <t>PÉRISCOLAIRE</t>
+  </si>
+  <si>
+    <t>DAYCARE OPERATION</t>
+  </si>
+  <si>
+    <t>FONCTIONNEMENT DE LA GARDERIE</t>
+  </si>
+  <si>
+    <t>DAYCARE ORGANIZATION</t>
+  </si>
+  <si>
+    <t>ORGANISATION DE LA GARDERIE</t>
+  </si>
+  <si>
+    <t>CULTURAL AND SPORTING ACTIVITIES</t>
+  </si>
+  <si>
+    <t>ACTIVITÉS CULTURELLE ET SPORTIVE</t>
+  </si>
+  <si>
+    <t>FRENCH</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>ANGLAIS</t>
+  </si>
+  <si>
+    <t>FRANCAIS</t>
+  </si>
+  <si>
+    <t>ESTABLISHMENT</t>
+  </si>
+  <si>
+    <t>ÉTABLISSEMENT</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>LANGUE</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>ACCEUIL</t>
   </si>
 </sst>
 </file>
@@ -486,15 +723,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AC5A95-E616-4CDB-8AF3-C426813B674E}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -510,40 +747,40 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -554,7 +791,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -565,13 +802,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -582,7 +819,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -604,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -620,13 +857,310 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>